<commit_message>
changes to the UI
</commit_message>
<xml_diff>
--- a/expenses.xlsx
+++ b/expenses.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -495,6 +495,66 @@
         <v>19.97</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>06-28-2024</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Shopping</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>42.98</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>06-28-2024</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Shopping</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>57.29</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>06-28-2024</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Shopping</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>70.48</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>06-28-2024</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Shopping</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>33.02</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>